<commit_message>
updated source doc and deleted rr file.
</commit_message>
<xml_diff>
--- a/Source.xlsx
+++ b/Source.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDC11DC-66E0-44E0-BC8B-EE454F122198}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BC2381-9332-4882-BFBC-AA8CB32E858A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Android studio " sheetId="1" r:id="rId1"/>
@@ -23,12 +23,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>GIT  BASH</t>
+  </si>
+  <si>
+    <t>GIT GUI</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch creation for local  </t>
+  </si>
+  <si>
+    <t>Commit and Push</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch selection if not in required branch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pull </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the current branch before pull                  Remote-&gt;Fetch from-&gt;Origin.                             Merge-&gt; Local Merge-&gt;select tracking branch-&gt;Merge.                </t>
+  </si>
+  <si>
+    <t>Branch-&gt; checkout-&gt;select local branch-&gt;choose required branch-&gt; checkout.</t>
+  </si>
+  <si>
+    <t>Rescan-&gt; click stage changed-&gt; commit-&gt; push.</t>
+  </si>
+  <si>
+    <t>Branch-&gt;Give Name-&gt;select tracking branch-&gt; select required branch-&gt; create.</t>
+  </si>
+  <si>
+    <t>Add extra functionalities</t>
+  </si>
+  <si>
+    <t>Tools-&gt;Add-&gt;function name-&gt;enter command-&gt; Add.</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -36,16 +85,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -53,12 +116,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,9 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -382,12 +471,109 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFAEF3DF-5FE5-4374-8B74-248D3EAA1C71}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="E9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="E11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added chat box and included message activity.
</commit_message>
<xml_diff>
--- a/Source.xlsx
+++ b/Source.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BC2381-9332-4882-BFBC-AA8CB32E858A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F175BB-8B87-4484-9C42-009391E591FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Android studio " sheetId="1" r:id="rId1"/>
-    <sheet name="Firebase" sheetId="2" r:id="rId2"/>
-    <sheet name="Gradle" sheetId="3" r:id="rId3"/>
-    <sheet name="GitHub" sheetId="4" r:id="rId4"/>
+    <sheet name="Tasks" sheetId="5" r:id="rId2"/>
+    <sheet name="Firebase" sheetId="2" r:id="rId3"/>
+    <sheet name="Gradle" sheetId="3" r:id="rId4"/>
+    <sheet name="GitHub" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Command</t>
   </si>
@@ -71,6 +72,57 @@
   </si>
   <si>
     <t>Tools-&gt;Add-&gt;function name-&gt;enter command-&gt; Add.</t>
+  </si>
+  <si>
+    <t>Gradle Dependencies to note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    implementation 'com.fasterxml.jackson.core:jackson-core:2.10.2'
+    implementation 'com.fasterxml.jackson.core:jackson-annotations:2.10.2'
+    implementation 'com.fasterxml.jackson.core:jackson-databind:2.10.2'</t>
+  </si>
+  <si>
+    <t>Usage purpose</t>
+  </si>
+  <si>
+    <t>For object mapper i.e to conver object to any type of collections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    implementation 'com.google.android.material:material:1.1.0'</t>
+  </si>
+  <si>
+    <t>Material design to support some ui functions such as Chip etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    implementation 'com.google.android.gms:play-services-auth:16.0.1'</t>
+  </si>
+  <si>
+    <t>Google sign up dependencies.</t>
+  </si>
+  <si>
+    <t>Configuration settings/errors faced</t>
+  </si>
+  <si>
+    <t>Google sign in we need to add SHA1 finger print in the project settings to enable G sign up.</t>
+  </si>
+  <si>
+    <t>Pending Tasks</t>
+  </si>
+  <si>
+    <t>Floating Tasks</t>
+  </si>
+  <si>
+    <t>Developer name</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error status </t>
+  </si>
+  <si>
+    <t>Descprition</t>
   </si>
 </sst>
 </file>
@@ -135,21 +187,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -446,34 +503,132 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758BC84F-11D0-48F3-B318-71B716B5A7DB}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E8E7D2E-83DF-4177-BD14-E1FAB1BDD632}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD985C6-88C6-43E4-9B89-18D242B51D22}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758BC84F-11D0-48F3-B318-71B716B5A7DB}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="76.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD985C6-88C6-43E4-9B89-18D242B51D22}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="83.90625" customWidth="1"/>
+    <col min="2" max="2" width="54.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFAEF3DF-5FE5-4374-8B74-248D3EAA1C71}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -492,23 +647,23 @@
       <c r="B1" s="6"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>